<commit_message>
Updated lit review with D. medinensis
</commit_message>
<xml_diff>
--- a/lit review master.xlsx
+++ b/lit review master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineschluth/bansallab/humanhelminths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44B4E977-9F10-D643-8501-DCDA60DAD627}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7FB9B9D-8612-D64A-857E-7AD91BEFE950}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{91FD2FA6-0E6B-461F-B49B-24525378B928}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="199">
   <si>
     <t>Latin name</t>
   </si>
@@ -648,9 +648,6 @@
     <t>Eastern Zambia</t>
   </si>
   <si>
-    <t>Community-based study</t>
-  </si>
-  <si>
     <t>https://journals.plos.org/plosntds/article?id=10.1371/journal.pntd.0001594</t>
   </si>
   <si>
@@ -685,9 +682,6 @@
   </si>
   <si>
     <t>Spatial cluster analysis</t>
-  </si>
-  <si>
-    <t>Spatial cluster analysis, use of mortality data</t>
   </si>
   <si>
     <t>ArcGIS, SaTScan, SAS 9.3, Epi Info 6</t>
@@ -1323,61 +1317,6 @@
     <t>Sub-Saharan Africa</t>
   </si>
   <si>
-    <t>Guinea</t>
-  </si>
-  <si>
-    <t>https://parasitesandvectors.biomedcentral.com/track/pdf/10.1186/s13071-015-1077-x</t>
-  </si>
-  <si>
-    <t>ICT, STATA, ArcGIS</t>
-  </si>
-  <si>
-    <r>
-      <t>Kouassi, Bernard L., Dziedzom K. de Souza, Andre Goepogui, Charles A. Narh, Sandra A. King, Baldé S. Mamadou, Lamia Diakité et al. "Assessing the presence of Wuchereria bancrofti in vector and human populations from urban communities in Conakry, Guinea." </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="5"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Parasites &amp; vectors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="5"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> 8, no. 1 (2015): 492.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This study found no cases of LF in the area. Do we still want to consider where human helminthiasis is </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri "/>
-      </rPr>
-      <t>not</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri "/>
-      </rPr>
-      <t>?</t>
-    </r>
-  </si>
-  <si>
     <t>https://onlinelibrary.wiley.com/doi/full/10.1111/j.1365-3156.2005.01558.x</t>
   </si>
   <si>
@@ -1549,14 +1488,231 @@
     <t>Ethiopia</t>
   </si>
   <si>
-    <t>https://journals.plos.org/plosntds/article?id=10.1371/journal.pntd.0006325</t>
+    <t>Dracunculus medinensis</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3886430/</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>No sample size given. Surveys conducted and geographic data collected but no specific methodologies mentioned. Check supplement?</t>
+  </si>
+  <si>
+    <r>
+      <t>Eberhard, M. L., Ruiz-Tiben, E., Hopkins, D. R., Farrell, C., Toe, F., Weiss, A., Withers, P. C., Jenks, M. H., Thiele, E. A., Cotton, J. A., Hance, Z., Holroyd, N., Cama, V. A., Tahir, M. A., … Mounda, T. (2014). The peculiar epidemiology of dracunculiasis in Chad. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The American journal of tropical medicine and hygiene</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>90</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1), 61-70.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5582630/</t>
+  </si>
+  <si>
+    <t>Systematic literature review</t>
+  </si>
+  <si>
+    <t>PubMed, WHO, CDC, Google Scholar</t>
+  </si>
+  <si>
+    <t>Check supplement for search terms used</t>
+  </si>
+  <si>
+    <r>
+      <t>Beyene, H. B., Bekele, A., Shifara, A., Ebstie, Y. A., Desalegn, Z., Kebede, Z., Mulugeta, A., Deribe, K., Tadesse, Z., Abebe, T., Kebede, B., Abrha, G., … Jima, D. (2017). Elimination of Guinea Worm Disease in Ethiopia; Current Status of the Disease's, Eradication Strategies and Challenges to the End Game. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ethiopian medical journal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Suppl 1), 15-31.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3748487/</t>
+  </si>
+  <si>
+    <t>South Sudan, Chad, Mali, Ethiopia</t>
+  </si>
+  <si>
+    <t>*DID NOT COME UP IN SEARCH* Map only present for South Sudan</t>
+  </si>
+  <si>
+    <t>Review of WHO initiative</t>
+  </si>
+  <si>
+    <r>
+      <t>Hopkins, D. R., Ruiz-Tiben, E., Weiss, A., Withers, P. C., Eberhard, M. L., &amp; Roy, S. L. (2013). Dracunculiasis eradication: and now, South Sudan. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The American journal of tropical medicine and hygiene</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>89</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(1), 5-10.</t>
+    </r>
+  </si>
+  <si>
+    <t>Review of disease control efforts</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2729080/</t>
+  </si>
+  <si>
+    <r>
+      <t>Rumunu, J., Brooker, S., Hopkins, A., Chane, F., Emerson, P., &amp; Kolaczinski, J. (2009). Southern Sudan: an opportunity for NTD control and elimination?. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Trends in parasitology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF303030"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(7), 301-7.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1664,6 +1820,26 @@
       <color rgb="FF333333"/>
       <name val="Calibri "/>
     </font>
+    <font>
+      <sz val="5"/>
+      <color rgb="FF303030"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="5"/>
+      <color rgb="FF303030"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1686,7 +1862,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1714,6 +1890,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2029,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6841491-4DF6-412B-93BA-008054BB3AC1}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="135" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="135" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -2058,7 +2236,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2272,22 +2450,22 @@
         <v>44</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="12">
         <v>2012</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>73</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H9" s="4">
         <v>720</v>
@@ -2307,7 +2485,7 @@
         <v>70</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>68</v>
@@ -2376,83 +2554,83 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C13" s="12">
         <v>1998</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F13" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="H13" s="4">
         <v>130</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C14" s="12">
         <v>2002</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="H14" s="4">
         <v>79</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" s="12">
         <v>2003</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H15" s="4">
         <v>2219</v>
@@ -2460,51 +2638,51 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C16" s="12">
         <v>2005</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C17" s="12">
         <v>2011</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>68</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H17" s="4">
         <v>8670</v>
@@ -2512,25 +2690,25 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C18" s="12">
         <v>2012</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H18" s="4">
         <v>9288</v>
@@ -2538,54 +2716,54 @@
     </row>
     <row r="19" spans="1:11" ht="14" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C19" s="12">
         <v>2013</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C20" s="12">
         <v>2014</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="H20" s="4">
         <v>807</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2619,28 +2797,28 @@
         <v>8</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C22" s="12">
         <v>2012</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="H22" s="4">
         <v>2639</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="18" customHeight="1">
@@ -2677,25 +2855,25 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="C24" s="12">
         <v>2010</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="H24" s="4">
         <v>91</v>
@@ -2703,31 +2881,31 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C25" s="11">
         <v>2011</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H25" s="4">
         <v>17533</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2735,22 +2913,22 @@
         <v>44</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C26" s="11">
         <v>2017</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H26" s="4">
         <v>1420</v>
@@ -2761,25 +2939,25 @@
         <v>44</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C27" s="11">
         <v>2012</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2787,48 +2965,48 @@
         <v>44</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C28" s="11">
         <v>2015</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="K28" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C29" s="11">
         <v>2012</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F29" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="H29" s="4">
         <v>34294</v>
@@ -2836,25 +3014,25 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C30" s="11">
         <v>2014</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="H30" s="4">
         <v>9964</v>
@@ -2862,204 +3040,259 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C31" s="11">
         <v>2015</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H31" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C32" s="11">
-        <v>2015</v>
+        <v>2006</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="K32" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="H32" s="4">
-        <v>611</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C33" s="11">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>167</v>
+      <c r="H33" s="4">
+        <v>1073</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C34" s="11">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H34" s="4">
-        <v>1073</v>
+        <v>10943</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C35" s="11">
-        <v>2015</v>
+        <v>2006</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>87</v>
+        <v>170</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H35" s="4">
-        <v>10943</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C36" s="11">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>177</v>
+        <v>85</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>145</v>
+        <v>174</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H36" s="4">
-        <v>3600</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" s="15" t="s">
         <v>184</v>
       </c>
       <c r="C37" s="11">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="I37" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H37" s="4">
-        <v>1242</v>
-      </c>
     </row>
     <row r="38" spans="1:11">
+      <c r="A38" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>189</v>
+      </c>
       <c r="C38" s="11">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D38" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>186</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H38" s="4">
-        <v>18254</v>
+        <v>178</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="11">
+        <v>2013</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C40" s="11">
+        <v>2009</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>